<commit_message>
replaced all with updated files
</commit_message>
<xml_diff>
--- a/data/Epidemics Timeline.xlsx
+++ b/data/Epidemics Timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hitapadm-my.sharepoint.com/personal/brandon_c_hitap_net/Documents/Desktop/Comission work with Paula/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulachristen/Documents/idm_lit_review_3/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="334" documentId="11_F25DC773A252ABDACC10483891194EC25BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE4F75E8-E743-43EC-BD82-C713254AAEF1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8337B0AF-E0AB-1E41-8744-B3D347D31753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6020" yWindow="760" windowWidth="22740" windowHeight="18040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Year pathogen Location" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
     <author>tc={606B517D-2D6C-46B3-9341-5A52962E0929}</author>
   </authors>
   <commentList>
-    <comment ref="J116" authorId="0" shapeId="0" xr:uid="{606B517D-2D6C-46B3-9341-5A52962E0929}">
+    <comment ref="I116" authorId="0" shapeId="0" xr:uid="{606B517D-2D6C-46B3-9341-5A52962E0929}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
   <si>
     <t>Start year</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>Russian flu pandemic (H1N1)</t>
+  </si>
+  <si>
+    <t>H1N1 Russian Flu</t>
   </si>
 </sst>
 </file>
@@ -583,7 +586,7 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="J116" dT="2024-12-12T11:07:03.13" personId="{386ADF99-AEE3-46E7-B5FD-263CE8D01FE8}" id="{606B517D-2D6C-46B3-9341-5A52962E0929}">
+  <threadedComment ref="I116" dT="2024-12-12T11:07:03.13" personId="{386ADF99-AEE3-46E7-B5FD-263CE8D01FE8}" id="{606B517D-2D6C-46B3-9341-5A52962E0929}">
     <text xml:space="preserve">Verified 2013 mers still active
 </text>
   </threadedComment>
@@ -598,24 +601,24 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.90625" customWidth="1"/>
-    <col min="3" max="3" width="23.08984375" customWidth="1"/>
-    <col min="4" max="4" width="67.1796875" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" customWidth="1"/>
+    <col min="4" max="4" width="67.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -629,7 +632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <v>1894</v>
       </c>
@@ -643,7 +646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1899</v>
       </c>
@@ -657,7 +660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>1918</v>
       </c>
@@ -671,7 +674,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>1957</v>
       </c>
@@ -685,7 +688,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>1961</v>
       </c>
@@ -699,7 +702,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>1968</v>
       </c>
@@ -713,7 +716,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
         <v>1976</v>
       </c>
@@ -727,7 +730,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>1981</v>
       </c>
@@ -741,7 +744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>2002</v>
       </c>
@@ -755,7 +758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>2009</v>
       </c>
@@ -769,7 +772,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>2012</v>
       </c>
@@ -783,7 +786,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>2014</v>
       </c>
@@ -797,7 +800,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>2015</v>
       </c>
@@ -811,7 +814,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>2014</v>
       </c>
@@ -825,7 +828,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>2014</v>
       </c>
@@ -839,7 +842,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>2000</v>
       </c>
@@ -853,7 +856,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>2017</v>
       </c>
@@ -867,7 +870,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>2018</v>
       </c>
@@ -881,7 +884,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>2015</v>
       </c>
@@ -895,7 +898,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>2019</v>
       </c>
@@ -909,7 +912,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>2022</v>
       </c>
@@ -923,13 +926,13 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="5"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="C28" s="6" t="s">
         <v>36</v>
       </c>
@@ -937,7 +940,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="C29" s="6" t="s">
         <v>37</v>
       </c>
@@ -953,23 +956,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C38CD4-8F09-4C03-B158-03EB077BF6EF}">
-  <dimension ref="A1:O127"/>
+  <dimension ref="A1:N127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="G120" sqref="G120"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="6" width="14.54296875" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" customWidth="1"/>
-    <col min="8" max="8" width="14.6328125" customWidth="1"/>
-    <col min="9" max="9" width="12.6328125" customWidth="1"/>
-    <col min="10" max="11" width="8.7265625" customWidth="1"/>
+    <col min="2" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="5" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="10" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
@@ -977,43 +980,40 @@
         <v>9</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>41</v>
+      <c r="E1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1899</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1056,11 +1056,8 @@
       <c r="N2">
         <v>0</v>
       </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1900</v>
       </c>
@@ -1071,7 +1068,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1103,11 +1100,8 @@
       <c r="N3">
         <v>0</v>
       </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1901</v>
       </c>
@@ -1118,7 +1112,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1150,11 +1144,8 @@
       <c r="N4">
         <v>0</v>
       </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1902</v>
       </c>
@@ -1165,7 +1156,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1197,11 +1188,8 @@
       <c r="N5">
         <v>0</v>
       </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1903</v>
       </c>
@@ -1212,7 +1200,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1244,11 +1232,8 @@
       <c r="N6">
         <v>0</v>
       </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>1904</v>
       </c>
@@ -1259,7 +1244,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1291,11 +1276,8 @@
       <c r="N7">
         <v>0</v>
       </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>1905</v>
       </c>
@@ -1306,7 +1288,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1338,11 +1320,8 @@
       <c r="N8">
         <v>0</v>
       </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>1906</v>
       </c>
@@ -1353,7 +1332,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1385,11 +1364,8 @@
       <c r="N9">
         <v>0</v>
       </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>1907</v>
       </c>
@@ -1400,7 +1376,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1432,11 +1408,8 @@
       <c r="N10">
         <v>0</v>
       </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>1908</v>
       </c>
@@ -1447,7 +1420,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1479,11 +1452,8 @@
       <c r="N11">
         <v>0</v>
       </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>1909</v>
       </c>
@@ -1494,7 +1464,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1526,11 +1496,8 @@
       <c r="N12">
         <v>0</v>
       </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>1910</v>
       </c>
@@ -1541,7 +1508,7 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1573,11 +1540,8 @@
       <c r="N13">
         <v>0</v>
       </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>1911</v>
       </c>
@@ -1588,7 +1552,7 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1620,11 +1584,8 @@
       <c r="N14">
         <v>0</v>
       </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>1912</v>
       </c>
@@ -1635,7 +1596,7 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1667,11 +1628,8 @@
       <c r="N15">
         <v>0</v>
       </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>1913</v>
       </c>
@@ -1682,7 +1640,7 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1714,11 +1672,8 @@
       <c r="N16">
         <v>0</v>
       </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>1914</v>
       </c>
@@ -1729,7 +1684,7 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1761,11 +1716,8 @@
       <c r="N17">
         <v>0</v>
       </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>1915</v>
       </c>
@@ -1776,7 +1728,7 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1808,11 +1760,8 @@
       <c r="N18">
         <v>0</v>
       </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>1916</v>
       </c>
@@ -1823,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1855,11 +1804,8 @@
       <c r="N19">
         <v>0</v>
       </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>1917</v>
       </c>
@@ -1870,7 +1816,7 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1902,11 +1848,8 @@
       <c r="N20">
         <v>0</v>
       </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>1918</v>
       </c>
@@ -1917,7 +1860,7 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1949,11 +1892,8 @@
       <c r="N21">
         <v>0</v>
       </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>1919</v>
       </c>
@@ -1964,7 +1904,7 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1996,11 +1936,8 @@
       <c r="N22">
         <v>0</v>
       </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>1920</v>
       </c>
@@ -2011,7 +1948,7 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -2043,11 +1980,8 @@
       <c r="N23">
         <v>0</v>
       </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>1921</v>
       </c>
@@ -2058,7 +1992,7 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -2090,11 +2024,8 @@
       <c r="N24">
         <v>0</v>
       </c>
-      <c r="O24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>1922</v>
       </c>
@@ -2105,7 +2036,7 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -2137,11 +2068,8 @@
       <c r="N25">
         <v>0</v>
       </c>
-      <c r="O25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>1923</v>
       </c>
@@ -2152,7 +2080,7 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -2184,11 +2112,8 @@
       <c r="N26">
         <v>0</v>
       </c>
-      <c r="O26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>1924</v>
       </c>
@@ -2199,7 +2124,7 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -2231,11 +2156,8 @@
       <c r="N27">
         <v>0</v>
       </c>
-      <c r="O27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>1925</v>
       </c>
@@ -2246,7 +2168,7 @@
         <v>0</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -2278,11 +2200,8 @@
       <c r="N28">
         <v>0</v>
       </c>
-      <c r="O28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>1926</v>
       </c>
@@ -2293,7 +2212,7 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -2325,11 +2244,8 @@
       <c r="N29">
         <v>0</v>
       </c>
-      <c r="O29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>1927</v>
       </c>
@@ -2340,7 +2256,7 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -2372,11 +2288,8 @@
       <c r="N30">
         <v>0</v>
       </c>
-      <c r="O30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>1928</v>
       </c>
@@ -2387,7 +2300,7 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -2419,11 +2332,8 @@
       <c r="N31">
         <v>0</v>
       </c>
-      <c r="O31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>1929</v>
       </c>
@@ -2434,7 +2344,7 @@
         <v>0</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -2466,11 +2376,8 @@
       <c r="N32">
         <v>0</v>
       </c>
-      <c r="O32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>1930</v>
       </c>
@@ -2481,7 +2388,7 @@
         <v>0</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -2513,11 +2420,8 @@
       <c r="N33">
         <v>0</v>
       </c>
-      <c r="O33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>1931</v>
       </c>
@@ -2528,7 +2432,7 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -2560,11 +2464,8 @@
       <c r="N34">
         <v>0</v>
       </c>
-      <c r="O34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>1932</v>
       </c>
@@ -2575,7 +2476,7 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -2607,11 +2508,8 @@
       <c r="N35">
         <v>0</v>
       </c>
-      <c r="O35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>1933</v>
       </c>
@@ -2622,7 +2520,7 @@
         <v>0</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -2654,11 +2552,8 @@
       <c r="N36">
         <v>0</v>
       </c>
-      <c r="O36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>1934</v>
       </c>
@@ -2669,7 +2564,7 @@
         <v>0</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -2701,11 +2596,8 @@
       <c r="N37">
         <v>0</v>
       </c>
-      <c r="O37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>1935</v>
       </c>
@@ -2716,7 +2608,7 @@
         <v>0</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -2748,11 +2640,8 @@
       <c r="N38">
         <v>0</v>
       </c>
-      <c r="O38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>1936</v>
       </c>
@@ -2763,7 +2652,7 @@
         <v>0</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -2795,11 +2684,8 @@
       <c r="N39">
         <v>0</v>
       </c>
-      <c r="O39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>1937</v>
       </c>
@@ -2810,7 +2696,7 @@
         <v>0</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -2842,11 +2728,8 @@
       <c r="N40">
         <v>0</v>
       </c>
-      <c r="O40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>1938</v>
       </c>
@@ -2857,7 +2740,7 @@
         <v>0</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -2889,11 +2772,8 @@
       <c r="N41">
         <v>0</v>
       </c>
-      <c r="O41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>1939</v>
       </c>
@@ -2904,7 +2784,7 @@
         <v>0</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -2936,11 +2816,8 @@
       <c r="N42">
         <v>0</v>
       </c>
-      <c r="O42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>1940</v>
       </c>
@@ -2951,7 +2828,7 @@
         <v>0</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -2983,11 +2860,8 @@
       <c r="N43">
         <v>0</v>
       </c>
-      <c r="O43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>1941</v>
       </c>
@@ -2998,7 +2872,7 @@
         <v>0</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -3030,11 +2904,8 @@
       <c r="N44">
         <v>0</v>
       </c>
-      <c r="O44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>1942</v>
       </c>
@@ -3045,7 +2916,7 @@
         <v>0</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -3077,11 +2948,8 @@
       <c r="N45">
         <v>0</v>
       </c>
-      <c r="O45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>1943</v>
       </c>
@@ -3092,7 +2960,7 @@
         <v>0</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -3124,11 +2992,8 @@
       <c r="N46">
         <v>0</v>
       </c>
-      <c r="O46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>1944</v>
       </c>
@@ -3139,7 +3004,7 @@
         <v>0</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -3171,11 +3036,8 @@
       <c r="N47">
         <v>0</v>
       </c>
-      <c r="O47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>1945</v>
       </c>
@@ -3186,7 +3048,7 @@
         <v>0</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -3218,11 +3080,8 @@
       <c r="N48">
         <v>0</v>
       </c>
-      <c r="O48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>1946</v>
       </c>
@@ -3233,7 +3092,7 @@
         <v>0</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -3265,11 +3124,8 @@
       <c r="N49">
         <v>0</v>
       </c>
-      <c r="O49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>1947</v>
       </c>
@@ -3280,7 +3136,7 @@
         <v>0</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -3312,11 +3168,8 @@
       <c r="N50">
         <v>0</v>
       </c>
-      <c r="O50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>1948</v>
       </c>
@@ -3327,7 +3180,7 @@
         <v>0</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -3359,11 +3212,8 @@
       <c r="N51">
         <v>0</v>
       </c>
-      <c r="O51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>1949</v>
       </c>
@@ -3374,7 +3224,7 @@
         <v>0</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E52">
         <v>0</v>
@@ -3406,11 +3256,8 @@
       <c r="N52">
         <v>0</v>
       </c>
-      <c r="O52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>1950</v>
       </c>
@@ -3421,7 +3268,7 @@
         <v>0</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -3453,11 +3300,8 @@
       <c r="N53">
         <v>0</v>
       </c>
-      <c r="O53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>1951</v>
       </c>
@@ -3468,7 +3312,7 @@
         <v>0</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -3500,11 +3344,8 @@
       <c r="N54">
         <v>0</v>
       </c>
-      <c r="O54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>1952</v>
       </c>
@@ -3515,7 +3356,7 @@
         <v>0</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -3547,11 +3388,8 @@
       <c r="N55">
         <v>0</v>
       </c>
-      <c r="O55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>1953</v>
       </c>
@@ -3562,7 +3400,7 @@
         <v>0</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -3594,11 +3432,8 @@
       <c r="N56">
         <v>0</v>
       </c>
-      <c r="O56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>1954</v>
       </c>
@@ -3609,7 +3444,7 @@
         <v>0</v>
       </c>
       <c r="D57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -3641,11 +3476,8 @@
       <c r="N57">
         <v>0</v>
       </c>
-      <c r="O57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>1955</v>
       </c>
@@ -3656,7 +3488,7 @@
         <v>0</v>
       </c>
       <c r="D58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -3688,11 +3520,8 @@
       <c r="N58">
         <v>0</v>
       </c>
-      <c r="O58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>1956</v>
       </c>
@@ -3703,7 +3532,7 @@
         <v>0</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -3735,11 +3564,8 @@
       <c r="N59">
         <v>0</v>
       </c>
-      <c r="O59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>1957</v>
       </c>
@@ -3750,7 +3576,7 @@
         <v>1</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -3782,11 +3608,8 @@
       <c r="N60">
         <v>0</v>
       </c>
-      <c r="O60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>1958</v>
       </c>
@@ -3797,7 +3620,7 @@
         <v>1</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -3829,11 +3652,8 @@
       <c r="N61">
         <v>0</v>
       </c>
-      <c r="O61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>1959</v>
       </c>
@@ -3844,7 +3664,7 @@
         <v>0</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -3876,11 +3696,8 @@
       <c r="N62">
         <v>0</v>
       </c>
-      <c r="O62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>1960</v>
       </c>
@@ -3891,7 +3708,7 @@
         <v>0</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -3923,11 +3740,8 @@
       <c r="N63">
         <v>0</v>
       </c>
-      <c r="O63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>1961</v>
       </c>
@@ -3938,7 +3752,7 @@
         <v>0</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -3970,11 +3784,8 @@
       <c r="N64">
         <v>0</v>
       </c>
-      <c r="O64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>1962</v>
       </c>
@@ -3985,7 +3796,7 @@
         <v>0</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -4017,11 +3828,8 @@
       <c r="N65">
         <v>0</v>
       </c>
-      <c r="O65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>1963</v>
       </c>
@@ -4032,7 +3840,7 @@
         <v>0</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E66">
         <v>0</v>
@@ -4064,11 +3872,8 @@
       <c r="N66">
         <v>0</v>
       </c>
-      <c r="O66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>1964</v>
       </c>
@@ -4079,7 +3884,7 @@
         <v>0</v>
       </c>
       <c r="D67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E67">
         <v>0</v>
@@ -4111,11 +3916,8 @@
       <c r="N67">
         <v>0</v>
       </c>
-      <c r="O67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>1965</v>
       </c>
@@ -4126,7 +3928,7 @@
         <v>0</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -4158,11 +3960,8 @@
       <c r="N68">
         <v>0</v>
       </c>
-      <c r="O68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>1966</v>
       </c>
@@ -4173,7 +3972,7 @@
         <v>0</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -4205,11 +4004,8 @@
       <c r="N69">
         <v>0</v>
       </c>
-      <c r="O69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>1967</v>
       </c>
@@ -4220,7 +4016,7 @@
         <v>0</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -4252,11 +4048,8 @@
       <c r="N70">
         <v>0</v>
       </c>
-      <c r="O70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>1968</v>
       </c>
@@ -4270,7 +4063,7 @@
         <v>1</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F71">
         <v>0</v>
@@ -4299,11 +4092,8 @@
       <c r="N71">
         <v>0</v>
       </c>
-      <c r="O71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>1969</v>
       </c>
@@ -4317,7 +4107,7 @@
         <v>1</v>
       </c>
       <c r="E72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F72">
         <v>0</v>
@@ -4346,11 +4136,8 @@
       <c r="N72">
         <v>0</v>
       </c>
-      <c r="O72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>1970</v>
       </c>
@@ -4361,7 +4148,7 @@
         <v>0</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E73">
         <v>0</v>
@@ -4393,11 +4180,8 @@
       <c r="N73">
         <v>0</v>
       </c>
-      <c r="O73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>1971</v>
       </c>
@@ -4408,7 +4192,7 @@
         <v>0</v>
       </c>
       <c r="D74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E74">
         <v>0</v>
@@ -4440,11 +4224,8 @@
       <c r="N74">
         <v>0</v>
       </c>
-      <c r="O74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>1972</v>
       </c>
@@ -4455,7 +4236,7 @@
         <v>0</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -4487,11 +4268,8 @@
       <c r="N75">
         <v>0</v>
       </c>
-      <c r="O75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>1973</v>
       </c>
@@ -4502,7 +4280,7 @@
         <v>0</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -4534,11 +4312,8 @@
       <c r="N76">
         <v>0</v>
       </c>
-      <c r="O76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>1974</v>
       </c>
@@ -4549,7 +4324,7 @@
         <v>0</v>
       </c>
       <c r="D77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E77">
         <v>0</v>
@@ -4581,11 +4356,8 @@
       <c r="N77">
         <v>0</v>
       </c>
-      <c r="O77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>1975</v>
       </c>
@@ -4596,7 +4368,7 @@
         <v>0</v>
       </c>
       <c r="D78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E78">
         <v>0</v>
@@ -4628,11 +4400,8 @@
       <c r="N78">
         <v>0</v>
       </c>
-      <c r="O78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>1976</v>
       </c>
@@ -4643,13 +4412,13 @@
         <v>0</v>
       </c>
       <c r="D79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -4675,11 +4444,8 @@
       <c r="N79">
         <v>0</v>
       </c>
-      <c r="O79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>1977</v>
       </c>
@@ -4690,13 +4456,13 @@
         <v>0</v>
       </c>
       <c r="D80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G80">
         <v>0</v>
@@ -4722,11 +4488,8 @@
       <c r="N80">
         <v>0</v>
       </c>
-      <c r="O80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>1978</v>
       </c>
@@ -4737,7 +4500,7 @@
         <v>0</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E81">
         <v>0</v>
@@ -4769,11 +4532,8 @@
       <c r="N81">
         <v>0</v>
       </c>
-      <c r="O81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>1979</v>
       </c>
@@ -4784,7 +4544,7 @@
         <v>0</v>
       </c>
       <c r="D82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -4816,11 +4576,8 @@
       <c r="N82">
         <v>0</v>
       </c>
-      <c r="O82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>1980</v>
       </c>
@@ -4831,7 +4588,7 @@
         <v>0</v>
       </c>
       <c r="D83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E83">
         <v>0</v>
@@ -4863,11 +4620,8 @@
       <c r="N83">
         <v>0</v>
       </c>
-      <c r="O83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>1981</v>
       </c>
@@ -4878,16 +4632,16 @@
         <v>0</v>
       </c>
       <c r="D84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E84">
         <v>0</v>
       </c>
       <c r="F84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H84">
         <v>0</v>
@@ -4910,11 +4664,8 @@
       <c r="N84">
         <v>0</v>
       </c>
-      <c r="O84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>1982</v>
       </c>
@@ -4925,16 +4676,16 @@
         <v>0</v>
       </c>
       <c r="D85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E85">
         <v>0</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H85">
         <v>0</v>
@@ -4957,11 +4708,8 @@
       <c r="N85">
         <v>0</v>
       </c>
-      <c r="O85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>1983</v>
       </c>
@@ -4972,16 +4720,16 @@
         <v>0</v>
       </c>
       <c r="D86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E86">
         <v>0</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H86">
         <v>0</v>
@@ -5004,11 +4752,8 @@
       <c r="N86">
         <v>0</v>
       </c>
-      <c r="O86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>1984</v>
       </c>
@@ -5019,16 +4764,16 @@
         <v>0</v>
       </c>
       <c r="D87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E87">
         <v>0</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H87">
         <v>0</v>
@@ -5051,11 +4796,8 @@
       <c r="N87">
         <v>0</v>
       </c>
-      <c r="O87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>1985</v>
       </c>
@@ -5066,16 +4808,16 @@
         <v>0</v>
       </c>
       <c r="D88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E88">
         <v>0</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H88">
         <v>0</v>
@@ -5098,11 +4840,8 @@
       <c r="N88">
         <v>0</v>
       </c>
-      <c r="O88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>1986</v>
       </c>
@@ -5113,16 +4852,16 @@
         <v>0</v>
       </c>
       <c r="D89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E89">
         <v>0</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H89">
         <v>0</v>
@@ -5145,11 +4884,8 @@
       <c r="N89">
         <v>0</v>
       </c>
-      <c r="O89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>1987</v>
       </c>
@@ -5160,16 +4896,16 @@
         <v>0</v>
       </c>
       <c r="D90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E90">
         <v>0</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H90">
         <v>0</v>
@@ -5192,11 +4928,8 @@
       <c r="N90">
         <v>0</v>
       </c>
-      <c r="O90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>1988</v>
       </c>
@@ -5207,16 +4940,16 @@
         <v>0</v>
       </c>
       <c r="D91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E91">
         <v>0</v>
       </c>
       <c r="F91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H91">
         <v>0</v>
@@ -5239,11 +4972,8 @@
       <c r="N91">
         <v>0</v>
       </c>
-      <c r="O91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>1989</v>
       </c>
@@ -5254,16 +4984,16 @@
         <v>0</v>
       </c>
       <c r="D92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E92">
         <v>0</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H92">
         <v>0</v>
@@ -5286,11 +5016,8 @@
       <c r="N92">
         <v>0</v>
       </c>
-      <c r="O92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>1990</v>
       </c>
@@ -5301,16 +5028,16 @@
         <v>0</v>
       </c>
       <c r="D93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E93">
         <v>0</v>
       </c>
       <c r="F93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H93">
         <v>0</v>
@@ -5333,11 +5060,8 @@
       <c r="N93">
         <v>0</v>
       </c>
-      <c r="O93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>1991</v>
       </c>
@@ -5348,16 +5072,16 @@
         <v>0</v>
       </c>
       <c r="D94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E94">
         <v>0</v>
       </c>
       <c r="F94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H94">
         <v>0</v>
@@ -5380,11 +5104,8 @@
       <c r="N94">
         <v>0</v>
       </c>
-      <c r="O94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>1992</v>
       </c>
@@ -5395,16 +5116,16 @@
         <v>0</v>
       </c>
       <c r="D95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E95">
         <v>0</v>
       </c>
       <c r="F95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H95">
         <v>0</v>
@@ -5427,11 +5148,8 @@
       <c r="N95">
         <v>0</v>
       </c>
-      <c r="O95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>1993</v>
       </c>
@@ -5442,16 +5160,16 @@
         <v>0</v>
       </c>
       <c r="D96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96">
         <v>0</v>
       </c>
       <c r="F96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H96">
         <v>0</v>
@@ -5474,11 +5192,8 @@
       <c r="N96">
         <v>0</v>
       </c>
-      <c r="O96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>1994</v>
       </c>
@@ -5489,16 +5204,16 @@
         <v>0</v>
       </c>
       <c r="D97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E97">
         <v>0</v>
       </c>
       <c r="F97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H97">
         <v>0</v>
@@ -5521,11 +5236,8 @@
       <c r="N97">
         <v>0</v>
       </c>
-      <c r="O97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>1995</v>
       </c>
@@ -5536,16 +5248,16 @@
         <v>0</v>
       </c>
       <c r="D98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E98">
         <v>0</v>
       </c>
       <c r="F98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H98">
         <v>0</v>
@@ -5568,11 +5280,8 @@
       <c r="N98">
         <v>0</v>
       </c>
-      <c r="O98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>1996</v>
       </c>
@@ -5583,16 +5292,16 @@
         <v>0</v>
       </c>
       <c r="D99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99">
         <v>0</v>
       </c>
       <c r="F99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H99">
         <v>0</v>
@@ -5615,11 +5324,8 @@
       <c r="N99">
         <v>0</v>
       </c>
-      <c r="O99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>1997</v>
       </c>
@@ -5630,16 +5336,16 @@
         <v>0</v>
       </c>
       <c r="D100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E100">
         <v>0</v>
       </c>
       <c r="F100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H100">
         <v>0</v>
@@ -5662,11 +5368,8 @@
       <c r="N100">
         <v>0</v>
       </c>
-      <c r="O100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>1998</v>
       </c>
@@ -5677,16 +5380,16 @@
         <v>0</v>
       </c>
       <c r="D101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E101">
         <v>0</v>
       </c>
       <c r="F101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H101">
         <v>0</v>
@@ -5709,11 +5412,8 @@
       <c r="N101">
         <v>0</v>
       </c>
-      <c r="O101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>1999</v>
       </c>
@@ -5724,16 +5424,16 @@
         <v>0</v>
       </c>
       <c r="D102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102">
         <v>0</v>
       </c>
       <c r="F102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H102">
         <v>0</v>
@@ -5756,11 +5456,8 @@
       <c r="N102">
         <v>0</v>
       </c>
-      <c r="O102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>2000</v>
       </c>
@@ -5771,16 +5468,16 @@
         <v>0</v>
       </c>
       <c r="D103">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E103">
         <v>0</v>
       </c>
       <c r="F103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G103">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H103">
         <v>0</v>
@@ -5792,10 +5489,10 @@
         <v>0</v>
       </c>
       <c r="K103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L103">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M103">
         <v>0</v>
@@ -5803,11 +5500,8 @@
       <c r="N103">
         <v>0</v>
       </c>
-      <c r="O103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>2001</v>
       </c>
@@ -5818,16 +5512,16 @@
         <v>0</v>
       </c>
       <c r="D104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E104">
         <v>0</v>
       </c>
       <c r="F104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H104">
         <v>0</v>
@@ -5850,11 +5544,8 @@
       <c r="N104">
         <v>0</v>
       </c>
-      <c r="O104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>2002</v>
       </c>
@@ -5865,19 +5556,19 @@
         <v>0</v>
       </c>
       <c r="D105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E105">
         <v>0</v>
       </c>
       <c r="F105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G105">
         <v>1</v>
       </c>
       <c r="H105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I105">
         <v>0</v>
@@ -5897,11 +5588,8 @@
       <c r="N105">
         <v>0</v>
       </c>
-      <c r="O105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>2003</v>
       </c>
@@ -5912,19 +5600,19 @@
         <v>0</v>
       </c>
       <c r="D106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E106">
         <v>0</v>
       </c>
       <c r="F106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G106">
         <v>1</v>
       </c>
       <c r="H106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I106">
         <v>0</v>
@@ -5944,11 +5632,8 @@
       <c r="N106">
         <v>0</v>
       </c>
-      <c r="O106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>2004</v>
       </c>
@@ -5959,16 +5644,16 @@
         <v>0</v>
       </c>
       <c r="D107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E107">
         <v>0</v>
       </c>
       <c r="F107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H107">
         <v>0</v>
@@ -5991,11 +5676,8 @@
       <c r="N107">
         <v>0</v>
       </c>
-      <c r="O107">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>2005</v>
       </c>
@@ -6006,16 +5688,16 @@
         <v>0</v>
       </c>
       <c r="D108">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E108">
         <v>0</v>
       </c>
       <c r="F108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G108">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H108">
         <v>0</v>
@@ -6038,11 +5720,8 @@
       <c r="N108">
         <v>0</v>
       </c>
-      <c r="O108">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>2006</v>
       </c>
@@ -6053,16 +5732,16 @@
         <v>0</v>
       </c>
       <c r="D109">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E109">
         <v>0</v>
       </c>
       <c r="F109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G109">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H109">
         <v>0</v>
@@ -6085,11 +5764,8 @@
       <c r="N109">
         <v>0</v>
       </c>
-      <c r="O109">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>2007</v>
       </c>
@@ -6100,16 +5776,16 @@
         <v>0</v>
       </c>
       <c r="D110">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E110">
         <v>0</v>
       </c>
       <c r="F110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G110">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H110">
         <v>0</v>
@@ -6132,11 +5808,8 @@
       <c r="N110">
         <v>0</v>
       </c>
-      <c r="O110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>2008</v>
       </c>
@@ -6147,16 +5820,16 @@
         <v>0</v>
       </c>
       <c r="D111">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E111">
         <v>0</v>
       </c>
       <c r="F111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G111">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H111">
         <v>0</v>
@@ -6179,11 +5852,8 @@
       <c r="N111">
         <v>0</v>
       </c>
-      <c r="O111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>2009</v>
       </c>
@@ -6194,22 +5864,22 @@
         <v>0</v>
       </c>
       <c r="D112">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E112">
         <v>0</v>
       </c>
       <c r="F112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G112">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I112">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J112">
         <v>0</v>
@@ -6226,11 +5896,8 @@
       <c r="N112">
         <v>0</v>
       </c>
-      <c r="O112">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>2010</v>
       </c>
@@ -6241,22 +5908,22 @@
         <v>0</v>
       </c>
       <c r="D113">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E113">
         <v>0</v>
       </c>
       <c r="F113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G113">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I113">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J113">
         <v>0</v>
@@ -6273,11 +5940,8 @@
       <c r="N113">
         <v>0</v>
       </c>
-      <c r="O113">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>2011</v>
       </c>
@@ -6288,16 +5952,16 @@
         <v>0</v>
       </c>
       <c r="D114">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E114">
         <v>0</v>
       </c>
       <c r="F114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G114">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H114">
         <v>0</v>
@@ -6320,11 +5984,8 @@
       <c r="N114">
         <v>0</v>
       </c>
-      <c r="O114">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>2012</v>
       </c>
@@ -6335,25 +5996,25 @@
         <v>0</v>
       </c>
       <c r="D115">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E115">
         <v>0</v>
       </c>
       <c r="F115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G115">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H115">
         <v>0</v>
       </c>
       <c r="I115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J115">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K115">
         <v>0</v>
@@ -6367,11 +6028,8 @@
       <c r="N115">
         <v>0</v>
       </c>
-      <c r="O115">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>2013</v>
       </c>
@@ -6382,25 +6040,25 @@
         <v>0</v>
       </c>
       <c r="D116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E116">
         <v>0</v>
       </c>
       <c r="F116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H116">
         <v>0</v>
       </c>
-      <c r="I116">
-        <v>0</v>
-      </c>
-      <c r="J116" s="8">
-        <v>1</v>
+      <c r="I116" s="8">
+        <v>1</v>
+      </c>
+      <c r="J116">
+        <v>0</v>
       </c>
       <c r="K116">
         <v>0</v>
@@ -6414,11 +6072,8 @@
       <c r="N116">
         <v>0</v>
       </c>
-      <c r="O116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>2014</v>
       </c>
@@ -6429,22 +6084,22 @@
         <v>0</v>
       </c>
       <c r="D117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E117">
         <v>0</v>
       </c>
       <c r="F117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H117">
         <v>0</v>
       </c>
       <c r="I117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J117">
         <v>1</v>
@@ -6453,7 +6108,7 @@
         <v>1</v>
       </c>
       <c r="L117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M117">
         <v>0</v>
@@ -6461,11 +6116,8 @@
       <c r="N117">
         <v>0</v>
       </c>
-      <c r="O117">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>2015</v>
       </c>
@@ -6476,43 +6128,40 @@
         <v>0</v>
       </c>
       <c r="D118">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E118">
         <v>0</v>
       </c>
       <c r="F118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G118">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H118">
         <v>0</v>
       </c>
       <c r="I118">
-        <v>0</v>
-      </c>
-      <c r="J118">
-        <v>1</v>
-      </c>
-      <c r="K118" s="8">
+        <v>1</v>
+      </c>
+      <c r="J118" s="8">
+        <v>1</v>
+      </c>
+      <c r="K118">
         <v>1</v>
       </c>
       <c r="L118">
         <v>1</v>
       </c>
       <c r="M118">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N118">
         <v>0</v>
       </c>
-      <c r="O118">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>2016</v>
       </c>
@@ -6523,16 +6172,16 @@
         <v>0</v>
       </c>
       <c r="D119">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E119">
         <v>0</v>
       </c>
       <c r="F119">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G119">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H119">
         <v>0</v>
@@ -6540,26 +6189,23 @@
       <c r="I119">
         <v>0</v>
       </c>
-      <c r="J119">
-        <v>0</v>
-      </c>
-      <c r="K119" s="8">
+      <c r="J119" s="8">
+        <v>1</v>
+      </c>
+      <c r="K119">
         <v>1</v>
       </c>
       <c r="L119">
         <v>1</v>
       </c>
       <c r="M119">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N119">
         <v>0</v>
       </c>
-      <c r="O119">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>2017</v>
       </c>
@@ -6570,16 +6216,16 @@
         <v>0</v>
       </c>
       <c r="D120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E120">
         <v>0</v>
       </c>
       <c r="F120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H120">
         <v>0</v>
@@ -6587,14 +6233,14 @@
       <c r="I120">
         <v>0</v>
       </c>
-      <c r="J120">
-        <v>0</v>
-      </c>
-      <c r="K120" s="8">
+      <c r="J120" s="8">
+        <v>1</v>
+      </c>
+      <c r="K120">
         <v>1</v>
       </c>
       <c r="L120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M120">
         <v>0</v>
@@ -6602,11 +6248,8 @@
       <c r="N120">
         <v>0</v>
       </c>
-      <c r="O120">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>2018</v>
       </c>
@@ -6617,16 +6260,16 @@
         <v>0</v>
       </c>
       <c r="D121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E121">
         <v>0</v>
       </c>
       <c r="F121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H121">
         <v>0</v>
@@ -6634,14 +6277,14 @@
       <c r="I121">
         <v>0</v>
       </c>
-      <c r="J121">
-        <v>0</v>
-      </c>
-      <c r="K121" s="8">
+      <c r="J121" s="8">
+        <v>1</v>
+      </c>
+      <c r="K121">
         <v>1</v>
       </c>
       <c r="L121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M121">
         <v>0</v>
@@ -6649,11 +6292,8 @@
       <c r="N121">
         <v>0</v>
       </c>
-      <c r="O121">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>2019</v>
       </c>
@@ -6664,16 +6304,16 @@
         <v>0</v>
       </c>
       <c r="D122">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E122">
         <v>0</v>
       </c>
       <c r="F122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G122">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H122">
         <v>0</v>
@@ -6681,26 +6321,23 @@
       <c r="I122">
         <v>0</v>
       </c>
-      <c r="J122">
-        <v>0</v>
-      </c>
-      <c r="K122" s="8">
-        <v>1</v>
+      <c r="J122" s="8">
+        <v>1</v>
+      </c>
+      <c r="K122">
+        <v>0</v>
       </c>
       <c r="L122">
         <v>0</v>
       </c>
       <c r="M122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N122">
-        <v>1</v>
-      </c>
-      <c r="O122">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>2020</v>
       </c>
@@ -6711,16 +6348,16 @@
         <v>0</v>
       </c>
       <c r="D123">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E123">
         <v>0</v>
       </c>
       <c r="F123">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G123">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H123">
         <v>0</v>
@@ -6728,26 +6365,23 @@
       <c r="I123">
         <v>0</v>
       </c>
-      <c r="J123">
-        <v>0</v>
-      </c>
-      <c r="K123" s="8">
-        <v>1</v>
+      <c r="J123" s="8">
+        <v>1</v>
+      </c>
+      <c r="K123">
+        <v>0</v>
       </c>
       <c r="L123">
         <v>0</v>
       </c>
       <c r="M123">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N123">
-        <v>1</v>
-      </c>
-      <c r="O123">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>2021</v>
       </c>
@@ -6758,16 +6392,16 @@
         <v>0</v>
       </c>
       <c r="D124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E124">
         <v>0</v>
       </c>
       <c r="F124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H124">
         <v>0</v>
@@ -6775,26 +6409,23 @@
       <c r="I124">
         <v>0</v>
       </c>
-      <c r="J124">
-        <v>0</v>
-      </c>
-      <c r="K124" s="8">
-        <v>1</v>
+      <c r="J124" s="8">
+        <v>1</v>
+      </c>
+      <c r="K124">
+        <v>0</v>
       </c>
       <c r="L124">
         <v>0</v>
       </c>
       <c r="M124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N124">
-        <v>1</v>
-      </c>
-      <c r="O124">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>2022</v>
       </c>
@@ -6805,16 +6436,16 @@
         <v>0</v>
       </c>
       <c r="D125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E125">
         <v>0</v>
       </c>
       <c r="F125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H125">
         <v>0</v>
@@ -6822,26 +6453,23 @@
       <c r="I125">
         <v>0</v>
       </c>
-      <c r="J125">
-        <v>0</v>
-      </c>
-      <c r="K125" s="8">
-        <v>1</v>
+      <c r="J125" s="8">
+        <v>1</v>
+      </c>
+      <c r="K125">
+        <v>0</v>
       </c>
       <c r="L125">
         <v>0</v>
       </c>
       <c r="M125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N125">
         <v>1</v>
       </c>
-      <c r="O125">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>2023</v>
       </c>
@@ -6852,16 +6480,16 @@
         <v>0</v>
       </c>
       <c r="D126">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E126">
         <v>0</v>
       </c>
       <c r="F126">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G126">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H126">
         <v>0</v>
@@ -6869,26 +6497,23 @@
       <c r="I126">
         <v>0</v>
       </c>
-      <c r="J126">
-        <v>0</v>
-      </c>
-      <c r="K126" s="8">
-        <v>1</v>
+      <c r="J126" s="8">
+        <v>1</v>
+      </c>
+      <c r="K126">
+        <v>0</v>
       </c>
       <c r="L126">
         <v>0</v>
       </c>
       <c r="M126">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N126">
         <v>1</v>
       </c>
-      <c r="O126">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
         <v>2024</v>
       </c>
@@ -6899,16 +6524,16 @@
         <v>0</v>
       </c>
       <c r="D127">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E127">
         <v>0</v>
       </c>
       <c r="F127">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G127">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H127">
         <v>0</v>
@@ -6916,11 +6541,11 @@
       <c r="I127">
         <v>0</v>
       </c>
-      <c r="J127">
-        <v>0</v>
-      </c>
-      <c r="K127" s="8">
-        <v>1</v>
+      <c r="J127" s="8">
+        <v>1</v>
+      </c>
+      <c r="K127">
+        <v>0</v>
       </c>
       <c r="L127">
         <v>0</v>
@@ -6929,9 +6554,6 @@
         <v>0</v>
       </c>
       <c r="N127">
-        <v>0</v>
-      </c>
-      <c r="O127">
         <v>0</v>
       </c>
     </row>

</xml_diff>